<commit_message>
MaJ pp - Verif solution
</commit_message>
<xml_diff>
--- a/Cv_Asymptotique_V0.xlsx
+++ b/Cv_Asymptotique_V0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a2d04f23f7faf3ef/Bureau/PROFESSIONAL/CANADA/5_Cours/H25_MEC8211/0_Devoir 1/MEC8211_projet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7FA6F00-DB51-4FE1-86F3-1FC0F904FB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C7FA6F00-DB51-4FE1-86F3-1FC0F904FB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDDC2D10-FD09-4291-A7A6-CCE6B1E1F328}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{71DE9E3B-8139-49A5-9447-BED9AD2841B0}"/>
   </bookViews>
@@ -145,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -178,7 +178,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4844,8 +4844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDAE1E0-98B5-4FCE-A9B9-8A3F08494FE5}">
   <dimension ref="B1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AB23" sqref="AB23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5009,6 +5009,10 @@
         <f>D3</f>
         <v>3.0154E-2</v>
       </c>
+      <c r="N23">
+        <f>AVERAGE(J21,J26)</f>
+        <v>2.5038499999999999</v>
+      </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B26" t="s">

</xml_diff>